<commit_message>
Remove temporary Excel lock file and add 'Consumables' category to Category model
</commit_message>
<xml_diff>
--- a/drugs new.xlsx
+++ b/drugs new.xlsx
@@ -1645,8 +1645,8 @@
   </sheetPr>
   <dimension ref="A1:R227"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C148" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L171" activeCellId="0" sqref="L171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1657,7 +1657,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="21.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="21.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.99"/>
@@ -7527,7 +7527,10 @@
       </c>
       <c r="L169" s="12"/>
       <c r="M169" s="4" t="n">
-        <v>3003</v>
+        <v>2860</v>
+      </c>
+      <c r="N169" s="6" t="n">
+        <v>46507</v>
       </c>
       <c r="O169" s="4" t="n">
         <v>1</v>
@@ -7596,7 +7599,7 @@
       </c>
       <c r="L171" s="12"/>
       <c r="M171" s="4" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="N171" s="6" t="n">
         <v>46022</v>
@@ -7627,9 +7630,7 @@
       <c r="J172" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="K172" s="12" t="n">
-        <v>650</v>
-      </c>
+      <c r="K172" s="12"/>
       <c r="L172" s="12"/>
       <c r="M172" s="4" t="n">
         <v>1000</v>
@@ -7740,7 +7741,7 @@
       </c>
       <c r="L175" s="12"/>
       <c r="M175" s="4" t="n">
-        <v>2600</v>
+        <v>1000</v>
       </c>
       <c r="N175" s="6" t="n">
         <v>45991</v>
@@ -7901,7 +7902,7 @@
       </c>
       <c r="L180" s="12"/>
       <c r="M180" s="4" t="n">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="N180" s="6" t="n">
         <v>46234</v>
@@ -7931,11 +7932,14 @@
         <v>50</v>
       </c>
       <c r="K181" s="12" t="n">
-        <v>4500</v>
+        <v>8700</v>
       </c>
       <c r="L181" s="12"/>
       <c r="M181" s="4" t="n">
-        <v>92</v>
+        <v>40</v>
+      </c>
+      <c r="N181" s="6" t="n">
+        <v>46173</v>
       </c>
       <c r="O181" s="4" t="n">
         <v>1</v>
@@ -7966,7 +7970,7 @@
       </c>
       <c r="L182" s="12"/>
       <c r="M182" s="4" t="n">
-        <v>1000</v>
+        <v>850</v>
       </c>
       <c r="N182" s="6" t="n">
         <v>46265</v>
@@ -8000,7 +8004,7 @@
       </c>
       <c r="L183" s="12"/>
       <c r="M183" s="4" t="n">
-        <v>340</v>
+        <v>10</v>
       </c>
       <c r="N183" s="6" t="n">
         <v>45930</v>
@@ -8130,11 +8134,11 @@
         <v>406</v>
       </c>
       <c r="K187" s="12" t="n">
-        <v>970</v>
+        <v>200</v>
       </c>
       <c r="L187" s="12"/>
       <c r="M187" s="4" t="n">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="N187" s="6" t="n">
         <v>46356</v>
@@ -8300,14 +8304,14 @@
         <v>272</v>
       </c>
       <c r="K192" s="12" t="n">
-        <v>900</v>
+        <v>850</v>
       </c>
       <c r="L192" s="12"/>
       <c r="M192" s="4" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="N192" s="6" t="n">
-        <v>45900</v>
+        <v>46295</v>
       </c>
       <c r="O192" s="4" t="n">
         <v>1</v>
@@ -8406,10 +8410,10 @@
       </c>
       <c r="L195" s="12"/>
       <c r="M195" s="4" t="n">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="N195" s="6" t="n">
-        <v>45658</v>
+        <v>45748</v>
       </c>
       <c r="O195" s="4" t="n">
         <v>1</v>
@@ -8504,14 +8508,14 @@
         <v>406</v>
       </c>
       <c r="K198" s="12" t="n">
-        <v>689</v>
+        <v>845</v>
       </c>
       <c r="L198" s="12"/>
       <c r="M198" s="4" t="n">
-        <v>530</v>
+        <v>495</v>
       </c>
       <c r="N198" s="6" t="n">
-        <v>46326</v>
+        <v>46387</v>
       </c>
       <c r="O198" s="4" t="n">
         <v>1</v>
@@ -8672,7 +8676,7 @@
       </c>
       <c r="L203" s="12"/>
       <c r="M203" s="4" t="n">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="N203" s="6" t="n">
         <v>46022</v>
@@ -8932,14 +8936,14 @@
         <v>406</v>
       </c>
       <c r="K211" s="12" t="n">
-        <v>900</v>
+        <v>7246</v>
       </c>
       <c r="L211" s="12"/>
       <c r="M211" s="4" t="n">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="N211" s="6" t="n">
-        <v>45596</v>
+        <v>46081</v>
       </c>
       <c r="O211" s="4" t="n">
         <v>1</v>
@@ -9028,14 +9032,14 @@
         <v>406</v>
       </c>
       <c r="K214" s="12" t="n">
-        <v>1875</v>
+        <v>5350</v>
       </c>
       <c r="L214" s="12"/>
       <c r="M214" s="4" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="N214" s="6" t="n">
-        <v>46446</v>
+        <v>46112</v>
       </c>
       <c r="O214" s="4" t="n">
         <v>1</v>
@@ -9092,14 +9096,14 @@
         <v>272</v>
       </c>
       <c r="K216" s="12" t="n">
-        <v>9834</v>
+        <v>18686</v>
       </c>
       <c r="L216" s="12"/>
       <c r="M216" s="4" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N216" s="6" t="n">
-        <v>46142</v>
+        <v>45777</v>
       </c>
       <c r="O216" s="4" t="n">
         <v>1</v>
@@ -9194,7 +9198,7 @@
       </c>
       <c r="L219" s="12"/>
       <c r="M219" s="4" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="N219" s="6" t="n">
         <v>46081</v>
@@ -9260,7 +9264,7 @@
       </c>
       <c r="L221" s="12"/>
       <c r="M221" s="4" t="n">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="N221" s="6" t="n">
         <v>45808</v>
@@ -9360,7 +9364,7 @@
       </c>
       <c r="L224" s="12"/>
       <c r="M224" s="4" t="n">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="N224" s="6" t="n">
         <v>45747</v>
@@ -9394,7 +9398,7 @@
       </c>
       <c r="L225" s="12"/>
       <c r="M225" s="4" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="N225" s="6" t="n">
         <v>46112</v>

</xml_diff>

<commit_message>
Update DrugAdminForm fields and enhance drug search filtering
</commit_message>
<xml_diff>
--- a/drugs new.xlsx
+++ b/drugs new.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="488">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -1106,6 +1106,9 @@
   </si>
   <si>
     <t xml:space="preserve">HALOTHANE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HALTHANE</t>
   </si>
   <si>
     <t xml:space="preserve">ANAESTHETIC</t>
@@ -1668,8 +1671,8 @@
   </sheetPr>
   <dimension ref="A1:Q271"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C242" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F269" activeCellId="0" sqref="F269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8916,8 +8919,11 @@
       <c r="D177" s="1" t="s">
         <v>361</v>
       </c>
+      <c r="F177" s="1" t="s">
+        <v>362</v>
+      </c>
       <c r="G177" s="5" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="H177" s="1" t="s">
         <v>300</v>
@@ -8947,13 +8953,13 @@
     </row>
     <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D178" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="F178" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="G178" s="5" t="s">
         <v>363</v>
-      </c>
-      <c r="F178" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="G178" s="5" t="s">
-        <v>362</v>
       </c>
       <c r="H178" s="1" t="s">
         <v>300</v>
@@ -8986,13 +8992,13 @@
     </row>
     <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D179" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="F179" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="G179" s="5" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="H179" s="1" t="s">
         <v>300</v>
@@ -9025,10 +9031,10 @@
     </row>
     <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D180" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="F180" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="G180" s="5" t="s">
         <v>237</v>
@@ -9190,19 +9196,19 @@
     </row>
     <row r="184" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D184" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="E184" s="1" t="s">
         <v>201</v>
       </c>
       <c r="F184" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="G184" s="5" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="H184" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="I184" s="1" t="s">
         <v>342</v>
@@ -9244,7 +9250,7 @@
         <v>44</v>
       </c>
       <c r="H185" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="I185" s="1" t="s">
         <v>342</v>
@@ -9313,19 +9319,19 @@
     </row>
     <row r="187" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D187" s="1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="E187" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="F187" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="F187" s="1" t="s">
-        <v>369</v>
-      </c>
       <c r="G187" s="5" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="H187" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="I187" s="1" t="s">
         <v>342</v>
@@ -9355,16 +9361,16 @@
     </row>
     <row r="188" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D188" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="F188" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="G188" s="5" t="s">
         <v>85</v>
       </c>
       <c r="H188" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="I188" s="1" t="s">
         <v>342</v>
@@ -9397,16 +9403,16 @@
         <v>180</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="F189" s="1" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="G189" s="5" t="s">
         <v>182</v>
       </c>
       <c r="H189" s="1" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="I189" s="1" t="s">
         <v>342</v>
@@ -9436,19 +9442,19 @@
     </row>
     <row r="190" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D190" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>271</v>
       </c>
       <c r="F190" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="G190" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H190" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="I190" s="1" t="s">
         <v>342</v>
@@ -9478,16 +9484,16 @@
     </row>
     <row r="191" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D191" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="F191" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="G191" s="5" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="H191" s="1" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="I191" s="1" t="s">
         <v>342</v>
@@ -9517,19 +9523,19 @@
     </row>
     <row r="192" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D192" s="1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="E192" s="10" t="n">
         <v>0.02</v>
       </c>
       <c r="F192" s="1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="G192" s="5" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="H192" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="I192" s="1" t="s">
         <v>342</v>
@@ -9559,16 +9565,16 @@
     </row>
     <row r="193" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D193" s="1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="F193" s="1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="G193" s="5" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="H193" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="I193" s="1" t="s">
         <v>342</v>
@@ -9598,13 +9604,13 @@
     </row>
     <row r="194" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D194" s="1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="F194" s="1" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="G194" s="5" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="H194" s="1" t="s">
         <v>76</v>
@@ -9637,16 +9643,16 @@
     </row>
     <row r="195" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D195" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="F195" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="G195" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="F195" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="G195" s="5" t="s">
-        <v>385</v>
-      </c>
       <c r="H195" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="I195" s="1" t="s">
         <v>342</v>
@@ -9676,13 +9682,13 @@
     </row>
     <row r="196" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D196" s="1" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="E196" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="F196" s="1" t="s">
         <v>389</v>
-      </c>
-      <c r="F196" s="1" t="s">
-        <v>388</v>
       </c>
       <c r="G196" s="5" t="s">
         <v>51</v>
@@ -9718,16 +9724,16 @@
     </row>
     <row r="197" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D197" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="F197" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="G197" s="5" t="s">
         <v>59</v>
       </c>
       <c r="H197" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="I197" s="1" t="s">
         <v>342</v>
@@ -9757,19 +9763,19 @@
     </row>
     <row r="198" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D198" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="E198" s="1" t="s">
         <v>130</v>
       </c>
       <c r="F198" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="G198" s="5" t="s">
         <v>162</v>
       </c>
       <c r="H198" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="I198" s="1" t="s">
         <v>342</v>
@@ -9799,16 +9805,16 @@
     </row>
     <row r="199" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D199" s="1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="F199" s="1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G199" s="5" t="s">
         <v>150</v>
       </c>
       <c r="H199" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="I199" s="1" t="s">
         <v>342</v>
@@ -9838,16 +9844,16 @@
     </row>
     <row r="200" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D200" s="1" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="F200" s="1" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="G200" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H200" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="I200" s="1" t="s">
         <v>342</v>
@@ -9877,16 +9883,16 @@
     </row>
     <row r="201" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D201" s="1" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="F201" s="1" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="G201" s="5" t="s">
         <v>150</v>
       </c>
       <c r="H201" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="I201" s="1" t="s">
         <v>342</v>
@@ -9916,16 +9922,16 @@
     </row>
     <row r="202" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D202" s="1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E202" s="1" t="s">
         <v>201</v>
       </c>
       <c r="F202" s="1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="G202" s="5" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="H202" s="1" t="s">
         <v>98</v>
@@ -9958,16 +9964,16 @@
     </row>
     <row r="203" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D203" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="E203" s="1" t="s">
         <v>204</v>
       </c>
       <c r="F203" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="G203" s="5" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="H203" s="1" t="s">
         <v>145</v>
@@ -10000,13 +10006,13 @@
     </row>
     <row r="204" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D204" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="F204" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="G204" s="5" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="H204" s="1" t="s">
         <v>32</v>
@@ -10039,13 +10045,13 @@
     </row>
     <row r="205" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D205" s="1" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="E205" s="1" t="s">
         <v>130</v>
       </c>
       <c r="F205" s="1" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="G205" s="5" t="s">
         <v>179</v>
@@ -10081,16 +10087,16 @@
     </row>
     <row r="206" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D206" s="1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="F206" s="1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="G206" s="5" t="s">
         <v>237</v>
       </c>
       <c r="H206" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="I206" s="1" t="s">
         <v>342</v>
@@ -10120,13 +10126,13 @@
     </row>
     <row r="207" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D207" s="1" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="E207" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="F207" s="1" t="s">
         <v>403</v>
-      </c>
-      <c r="F207" s="1" t="s">
-        <v>402</v>
       </c>
       <c r="G207" s="5" t="s">
         <v>182</v>
@@ -10162,16 +10168,16 @@
     </row>
     <row r="208" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D208" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="F208" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="G208" s="5" t="s">
         <v>179</v>
       </c>
       <c r="H208" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="I208" s="1" t="s">
         <v>342</v>
@@ -10201,16 +10207,16 @@
     </row>
     <row r="209" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D209" s="1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="F209" s="1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="G209" s="5" t="s">
         <v>237</v>
       </c>
       <c r="H209" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="I209" s="1" t="s">
         <v>342</v>
@@ -10240,10 +10246,10 @@
     </row>
     <row r="210" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D210" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="F210" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="G210" s="5" t="s">
         <v>59</v>
@@ -10279,16 +10285,16 @@
     </row>
     <row r="211" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D211" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="F211" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="G211" s="5" t="s">
         <v>162</v>
       </c>
       <c r="H211" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="I211" s="1" t="s">
         <v>342</v>
@@ -10318,16 +10324,16 @@
     </row>
     <row r="212" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D212" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F212" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="G212" s="5" t="s">
         <v>162</v>
       </c>
       <c r="H212" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="I212" s="1" t="s">
         <v>342</v>
@@ -10357,16 +10363,16 @@
     </row>
     <row r="213" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D213" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="F213" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="G213" s="5" t="s">
         <v>237</v>
       </c>
       <c r="H213" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="I213" s="1" t="s">
         <v>342</v>
@@ -10396,16 +10402,16 @@
     </row>
     <row r="214" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D214" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="F214" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="G214" s="5" t="s">
         <v>237</v>
       </c>
       <c r="H214" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="I214" s="1" t="s">
         <v>342</v>
@@ -10435,16 +10441,16 @@
     </row>
     <row r="215" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D215" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="F215" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="G215" s="5" t="s">
         <v>176</v>
       </c>
       <c r="H215" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="I215" s="1" t="s">
         <v>342</v>
@@ -10474,10 +10480,10 @@
     </row>
     <row r="216" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D216" s="1" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F216" s="1" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="G216" s="5" t="s">
         <v>51</v>
@@ -10513,13 +10519,13 @@
     </row>
     <row r="217" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D217" s="1" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="E217" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="F217" s="1" t="s">
         <v>417</v>
-      </c>
-      <c r="F217" s="1" t="s">
-        <v>416</v>
       </c>
       <c r="G217" s="5" t="s">
         <v>20</v>
@@ -10555,13 +10561,13 @@
     </row>
     <row r="218" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D218" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="F218" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="G218" s="5" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="H218" s="1" t="s">
         <v>183</v>
@@ -10594,13 +10600,13 @@
     </row>
     <row r="219" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D219" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="F219" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="G219" s="5" t="s">
         <v>420</v>
-      </c>
-      <c r="F219" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="G219" s="5" t="s">
-        <v>419</v>
       </c>
       <c r="H219" s="1" t="s">
         <v>183</v>
@@ -10636,13 +10642,13 @@
         <v>326</v>
       </c>
       <c r="F220" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G220" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H220" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="I220" s="1" t="s">
         <v>342</v>
@@ -10672,13 +10678,13 @@
     </row>
     <row r="221" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D221" s="1" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="F221" s="1" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="G221" s="5" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="H221" s="1" t="s">
         <v>64</v>
@@ -10711,13 +10717,13 @@
     </row>
     <row r="222" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D222" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="F222" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="G222" s="5" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="H222" s="1" t="s">
         <v>64</v>
@@ -10750,13 +10756,13 @@
     </row>
     <row r="223" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D223" s="1" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="F223" s="1" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="G223" s="5" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="I223" s="1" t="s">
         <v>342</v>
@@ -10786,13 +10792,13 @@
     </row>
     <row r="224" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D224" s="1" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="F224" s="1" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="G224" s="5" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="H224" s="1" t="s">
         <v>98</v>
@@ -10825,13 +10831,13 @@
     </row>
     <row r="225" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D225" s="1" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="F225" s="1" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="G225" s="5" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="H225" s="1" t="s">
         <v>98</v>
@@ -10864,16 +10870,16 @@
     </row>
     <row r="226" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D226" s="1" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="E226" s="1" t="s">
         <v>278</v>
       </c>
       <c r="F226" s="1" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="G226" s="5" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="H226" s="1" t="s">
         <v>183</v>
@@ -10906,10 +10912,10 @@
     </row>
     <row r="227" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D227" s="1" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F227" s="1" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G227" s="5" t="s">
         <v>51</v>
@@ -10945,13 +10951,13 @@
     </row>
     <row r="228" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D228" s="1" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="F228" s="1" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="G228" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H228" s="1" t="s">
         <v>64</v>
@@ -10978,13 +10984,13 @@
     </row>
     <row r="229" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D229" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F229" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="G229" s="1" t="s">
         <v>438</v>
-      </c>
-      <c r="F229" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="G229" s="1" t="s">
-        <v>437</v>
       </c>
       <c r="H229" s="1" t="s">
         <v>64</v>
@@ -11008,13 +11014,13 @@
     </row>
     <row r="230" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D230" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="F230" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G230" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H230" s="1" t="s">
         <v>64</v>
@@ -11041,13 +11047,13 @@
     </row>
     <row r="231" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D231" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="F231" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="G231" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H231" s="1" t="s">
         <v>64</v>
@@ -11074,13 +11080,13 @@
     </row>
     <row r="232" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D232" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="F232" s="1" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="G232" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H232" s="1" t="s">
         <v>64</v>
@@ -11107,13 +11113,13 @@
     </row>
     <row r="233" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D233" s="1" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="F233" s="1" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="G233" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H233" s="1" t="s">
         <v>64</v>
@@ -11140,13 +11146,13 @@
     </row>
     <row r="234" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D234" s="1" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="F234" s="1" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="G234" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H234" s="1" t="s">
         <v>64</v>
@@ -11173,13 +11179,13 @@
     </row>
     <row r="235" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D235" s="1" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="F235" s="1" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="G235" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H235" s="1" t="s">
         <v>64</v>
@@ -11206,13 +11212,13 @@
     </row>
     <row r="236" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D236" s="1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="F236" s="1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="G236" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H236" s="1" t="s">
         <v>64</v>
@@ -11239,13 +11245,13 @@
     </row>
     <row r="237" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D237" s="1" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="F237" s="1" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="G237" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H237" s="1" t="s">
         <v>64</v>
@@ -11272,13 +11278,13 @@
     </row>
     <row r="238" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D238" s="1" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F238" s="1" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="G238" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H238" s="1" t="s">
         <v>64</v>
@@ -11305,13 +11311,13 @@
     </row>
     <row r="239" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D239" s="1" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="F239" s="1" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="G239" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H239" s="1" t="s">
         <v>64</v>
@@ -11338,13 +11344,13 @@
     </row>
     <row r="240" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D240" s="1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="F240" s="1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="G240" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H240" s="1" t="s">
         <v>64</v>
@@ -11371,13 +11377,13 @@
     </row>
     <row r="241" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D241" s="1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="F241" s="1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="G241" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H241" s="1" t="s">
         <v>64</v>
@@ -11404,13 +11410,13 @@
     </row>
     <row r="242" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D242" s="1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="F242" s="1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="G242" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H242" s="1" t="s">
         <v>64</v>
@@ -11434,13 +11440,13 @@
     </row>
     <row r="243" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D243" s="1" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="F243" s="1" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="G243" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H243" s="1" t="s">
         <v>64</v>
@@ -11467,13 +11473,13 @@
     </row>
     <row r="244" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D244" s="1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="F244" s="1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="G244" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H244" s="1" t="s">
         <v>64</v>
@@ -11500,13 +11506,13 @@
     </row>
     <row r="245" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D245" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="F245" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="G245" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H245" s="1" t="s">
         <v>64</v>
@@ -11533,13 +11539,13 @@
     </row>
     <row r="246" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D246" s="1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="F246" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="G246" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H246" s="1" t="s">
         <v>64</v>
@@ -11566,13 +11572,13 @@
     </row>
     <row r="247" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D247" s="1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="F247" s="1" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="G247" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H247" s="1" t="s">
         <v>64</v>
@@ -11599,13 +11605,13 @@
     </row>
     <row r="248" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D248" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="F248" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="G248" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H248" s="1" t="s">
         <v>64</v>
@@ -11632,13 +11638,13 @@
     </row>
     <row r="249" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D249" s="1" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="F249" s="1" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="G249" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H249" s="1" t="s">
         <v>64</v>
@@ -11665,13 +11671,13 @@
     </row>
     <row r="250" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D250" s="1" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="F250" s="1" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="G250" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H250" s="1" t="s">
         <v>64</v>
@@ -11698,13 +11704,13 @@
     </row>
     <row r="251" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D251" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="F251" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="G251" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H251" s="1" t="s">
         <v>64</v>
@@ -11731,13 +11737,13 @@
     </row>
     <row r="252" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D252" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="F252" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="G252" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H252" s="1" t="s">
         <v>64</v>
@@ -11764,13 +11770,13 @@
     </row>
     <row r="253" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D253" s="1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="F253" s="1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="G253" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H253" s="1" t="s">
         <v>64</v>
@@ -11797,13 +11803,13 @@
     </row>
     <row r="254" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D254" s="1" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="F254" s="1" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="G254" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H254" s="1" t="s">
         <v>64</v>
@@ -11830,13 +11836,13 @@
     </row>
     <row r="255" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D255" s="1" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="F255" s="1" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="G255" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H255" s="1" t="s">
         <v>64</v>
@@ -11863,13 +11869,13 @@
     </row>
     <row r="256" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D256" s="1" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="F256" s="1" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="G256" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H256" s="1" t="s">
         <v>64</v>
@@ -11896,13 +11902,13 @@
     </row>
     <row r="257" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D257" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="F257" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="G257" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H257" s="1" t="s">
         <v>64</v>
@@ -11929,13 +11935,13 @@
     </row>
     <row r="258" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D258" s="1" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="F258" s="1" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="G258" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H258" s="1" t="s">
         <v>64</v>
@@ -11962,13 +11968,13 @@
     </row>
     <row r="259" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D259" s="1" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="F259" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="G259" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H259" s="1" t="s">
         <v>64</v>
@@ -11995,13 +12001,13 @@
     </row>
     <row r="260" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D260" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="F260" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="G260" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H260" s="1" t="s">
         <v>64</v>
@@ -12028,13 +12034,13 @@
     </row>
     <row r="261" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D261" s="1" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="F261" s="1" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="G261" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H261" s="1" t="s">
         <v>64</v>
@@ -12061,13 +12067,13 @@
     </row>
     <row r="262" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D262" s="1" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="F262" s="1" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="G262" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H262" s="1" t="s">
         <v>64</v>
@@ -12094,13 +12100,13 @@
     </row>
     <row r="263" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D263" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="F263" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="G263" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H263" s="1" t="s">
         <v>64</v>
@@ -12127,13 +12133,13 @@
     </row>
     <row r="264" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D264" s="1" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="F264" s="1" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="G264" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H264" s="1" t="s">
         <v>64</v>
@@ -12160,13 +12166,13 @@
     </row>
     <row r="265" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D265" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F265" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="G265" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H265" s="1" t="s">
         <v>64</v>
@@ -12193,13 +12199,13 @@
     </row>
     <row r="266" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D266" s="1" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="F266" s="1" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="G266" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H266" s="1" t="s">
         <v>64</v>
@@ -12226,13 +12232,13 @@
     </row>
     <row r="267" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D267" s="1" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="F267" s="1" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="G267" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H267" s="1" t="s">
         <v>64</v>
@@ -12259,13 +12265,13 @@
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D268" s="1" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="F268" s="1" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="G268" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="I268" s="1" t="s">
         <v>342</v>
@@ -12292,13 +12298,13 @@
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D269" s="1" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="F269" s="1" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="G269" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="I269" s="1" t="s">
         <v>342</v>
@@ -12337,7 +12343,7 @@
         <v>44</v>
       </c>
       <c r="H270" s="1" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="I270" s="1" t="s">
         <v>342</v>
@@ -12373,7 +12379,7 @@
         <v>345</v>
       </c>
       <c r="F271" s="1" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="G271" s="5" t="s">
         <v>97</v>

</xml_diff>